<commit_message>
* Update build script.
</commit_message>
<xml_diff>
--- a/example/BuildSchema/Tables/GameTable.xlsx
+++ b/example/BuildSchema/Tables/GameTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Devwinsoft\devarc\example\Builder\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Devwinsoft\devarc\example\BuildSchema\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76754DE-8F44-4D09-8F52-36365003DB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B4148F-8007-4F17-8E63-88A88545905E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
   </bookViews>
   <sheets>
     <sheet name="CHARACTER" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>charName</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -199,6 +199,14 @@
   </si>
   <si>
     <t>4,5,6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>errorTest</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -302,9 +310,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -342,7 +350,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -448,7 +456,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -590,7 +598,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -695,21 +703,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3401DA0E-6D94-4657-8FD9-3F778EFEE5A9}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -719,17 +727,17 @@
       <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -740,16 +748,19 @@
         <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -760,24 +771,27 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -787,17 +801,20 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>35</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -807,13 +824,16 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* Fix Devarc.Encrypt.  * Update BaseTable::GetClass() function.
</commit_message>
<xml_diff>
--- a/example/BuildSchema/Tables/GameTable.xlsx
+++ b/example/BuildSchema/Tables/GameTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Devwinsoft\devarc\example\BuildSchema\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B4148F-8007-4F17-8E63-88A88545905E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA2237D-CDBC-4B0E-AEF7-751C5CFC64B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>charName</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -202,11 +202,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>bool</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>errorTest</t>
+    <t>Account[]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>classTest</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -706,15 +706,17 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.75" customWidth="1"/>
+    <col min="7" max="7" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -727,10 +729,10 @@
       <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -748,13 +750,13 @@
         <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>37</v>
@@ -771,13 +773,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>36</v>
@@ -787,6 +789,9 @@
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>32</v>
       </c>
@@ -801,13 +806,10 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5">
+      <c r="D5">
         <v>10</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
         <v>35</v>
       </c>
       <c r="G5" t="s">
@@ -824,13 +826,10 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6">
+      <c r="D6">
         <v>20</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" t="s">
         <v>34</v>
       </c>
       <c r="G6" t="s">

</xml_diff>

<commit_message>
* Rename effect class names.  * Fix effect bugs.
</commit_message>
<xml_diff>
--- a/example/BuildSchema/Tables/GameTable.xlsx
+++ b/example/BuildSchema/Tables/GameTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Devwinsoft\devarc\example\BuildSchema\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA2237D-CDBC-4B0E-AEF7-751C5CFC64B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257F1E82-EAE7-4503-A476-31E22CC09A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
   </bookViews>
@@ -706,7 +706,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
* Update IDL and framework.
</commit_message>
<xml_diff>
--- a/example/BuildSchema/Tables/GameTable.xlsx
+++ b/example/BuildSchema/Tables/GameTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Devwinsoft\devarc\example\BuildSchema\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680AAE3B-EA07-415C-9938-D42C7294464A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6C6125-3E0E-4BAD-AC4E-331AC9CA11BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>charName</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -210,7 +210,23 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Test Field</t>
+    <t>Annotation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBigInt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cost</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.2, 30</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.1, 50</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -707,10 +723,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3401DA0E-6D94-4657-8FD9-3F778EFEE5A9}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -721,9 +737,11 @@
     <col min="5" max="5" width="12.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.75" customWidth="1"/>
     <col min="7" max="7" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.75" customWidth="1"/>
+    <col min="9" max="9" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -742,11 +760,11 @@
       <c r="G1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -768,8 +786,11 @@
       <c r="G2" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -791,8 +812,11 @@
       <c r="G3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -802,8 +826,11 @@
       <c r="F4" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -822,8 +849,11 @@
       <c r="G5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -841,6 +871,9 @@
       </c>
       <c r="G6" t="s">
         <v>40</v>
+      </c>
+      <c r="H6" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Add serialize/deserialize functions of CInt/CFloat.
</commit_message>
<xml_diff>
--- a/example/BuildSchema/Tables/GameTable.xlsx
+++ b/example/BuildSchema/Tables/GameTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Devwinsoft\devarc\example\BuildSchema\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6C6125-3E0E-4BAD-AC4E-331AC9CA11BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC50CD9B-4ED7-45F5-83EE-7890AB195E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
   <si>
     <t>charName</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -228,6 +228,21 @@
   <si>
     <t>1.1, 50</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CFloat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cFloat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cInt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CInt</t>
   </si>
 </sst>
 </file>
@@ -723,10 +738,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3401DA0E-6D94-4657-8FD9-3F778EFEE5A9}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -741,7 +756,7 @@
     <col min="9" max="9" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -764,7 +779,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -789,8 +804,14 @@
       <c r="H2" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -815,8 +836,14 @@
       <c r="H3" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -829,8 +856,14 @@
       <c r="H4" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -853,7 +886,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
* Update FSM classes.
</commit_message>
<xml_diff>
--- a/example/BuildSchema/Tables/GameTable.xlsx
+++ b/example/BuildSchema/Tables/GameTable.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Devwinsoft\devarc\example\BuildSchema\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D7AA05-CCEB-49F0-B958-29D791F5BF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6FAA10-70FC-48BB-9619-4F35462F53CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
+    <workbookView xWindow="1800" yWindow="780" windowWidth="25635" windowHeight="13905" activeTab="1" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
   </bookViews>
   <sheets>
     <sheet name="CHARACTER" sheetId="1" r:id="rId1"/>
+    <sheet name="BLOCK" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
   <si>
     <t>charName</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -72,6 +73,169 @@
   <si>
     <t>key,show</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>block_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>block_type</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>affect_list</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>icon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>string[]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>key</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>block_poison</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poison</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>affect_poison</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>icon_poison_1</t>
+  </si>
+  <si>
+    <t>block_dark_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dark</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>affect_dark</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>icon_dark_1</t>
+  </si>
+  <si>
+    <t>block_dark_2</t>
+  </si>
+  <si>
+    <t>block_dark_3</t>
+  </si>
+  <si>
+    <t>block_dark_4</t>
+  </si>
+  <si>
+    <t>block_ice_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ice</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>affect_ice</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>icon_ice_1</t>
+  </si>
+  <si>
+    <t>block_ice_2</t>
+  </si>
+  <si>
+    <t>block_ice_3</t>
+  </si>
+  <si>
+    <t>block_ice_4</t>
+  </si>
+  <si>
+    <t>block_fire_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fire</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>affect_fire</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>icon_fire_1</t>
+  </si>
+  <si>
+    <t>block_fire_2</t>
+  </si>
+  <si>
+    <t>block_fire_3</t>
+  </si>
+  <si>
+    <t>block_fire_4</t>
+  </si>
+  <si>
+    <t>block_heal_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>affect_heal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>icon_heal_1</t>
+  </si>
+  <si>
+    <t>block_heal_2</t>
+  </si>
+  <si>
+    <t>block_heal_3</t>
+  </si>
+  <si>
+    <t>block_heal_4</t>
+  </si>
+  <si>
+    <t>block_lightning_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lightning</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>affect_lightning</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>icon_air_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>block_lightning_2</t>
+  </si>
+  <si>
+    <t>block_lightning_3</t>
+  </si>
+  <si>
+    <t>icon_air_1</t>
+  </si>
+  <si>
+    <t>block_lightning_4</t>
   </si>
 </sst>
 </file>
@@ -485,7 +649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2E1AEE7-F4DE-4E91-91DE-1DBDA9BA8502}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -550,4 +714,352 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224FE3DD-26F3-4408-9460-F15DA3E4D170}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="18.75" customWidth="1"/>
+    <col min="4" max="4" width="26.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>